<commit_message>
Obtained transition matrix and eigenvectors
</commit_message>
<xml_diff>
--- a/IOBgamemap.xlsx
+++ b/IOBgamemap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Oliver/Desktop/NEU/IS6105/001443089_001498905_6_Zhe_Xu_Yixin_Guo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A00C6F-84A4-6443-9015-B301E6F3B068}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6652E342-346E-8B4B-BCDB-598DEFD4CE8F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{75293F48-95FD-CA44-BED8-E365127A4EB5}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>GO</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>Zombies will not go ahead of player, even though zombies' steps &gt; player's roll and zombies' position is &lt;= 2 cells away from player</t>
+  </si>
+  <si>
+    <t>Diagon Alley</t>
+  </si>
+  <si>
+    <t>Diagon Alley: 1/2 chance of player cannot find the way out (stuck in DA until player draw draw the card with "the key", then advances 1 cell), 1/2 chance of player advances 1 cell (draw "the key" card)</t>
+  </si>
+  <si>
+    <t>Chance cards: there are 2 chance cards, 1 of them is "the key" for the player to get out of Diagon Alley, the other one traps player for this current roll</t>
   </si>
 </sst>
 </file>
@@ -708,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21664577-9EB1-C540-B6C7-0882C76341D6}">
-  <dimension ref="A1:W26"/>
+  <dimension ref="A1:AP72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+      <selection activeCell="B30" sqref="B30:O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -724,28 +733,76 @@
     <col min="9" max="9" width="12.5" customWidth="1"/>
     <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="23" width="10.83203125" style="9"/>
+    <col min="14" max="14" width="10.83203125" style="9" customWidth="1"/>
+    <col min="15" max="23" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16"/>
+      <c r="C2" s="16">
+        <v>1</v>
+      </c>
       <c r="D2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
+      <c r="E2" s="16">
+        <v>2</v>
+      </c>
+      <c r="F2" s="17">
+        <v>3</v>
+      </c>
+      <c r="G2" s="16">
+        <v>4</v>
+      </c>
+      <c r="H2" s="17">
+        <v>5</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="16">
+        <v>7</v>
+      </c>
       <c r="K2" s="17" t="s">
         <v>3</v>
       </c>
@@ -753,8 +810,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B3" s="12"/>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>39</v>
+      </c>
+      <c r="B3" s="12">
+        <v>29</v>
+      </c>
       <c r="C3" s="18"/>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
@@ -764,9 +826,17 @@
       <c r="I3" s="19"/>
       <c r="J3" s="19"/>
       <c r="K3" s="20"/>
-      <c r="L3" s="14"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L3" s="14">
+        <v>8</v>
+      </c>
+      <c r="M3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>38</v>
+      </c>
       <c r="B4" s="13" t="s">
         <v>4</v>
       </c>
@@ -779,9 +849,17 @@
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="22"/>
-      <c r="L4" s="14"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L4" s="14">
+        <v>9</v>
+      </c>
+      <c r="M4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>37</v>
+      </c>
       <c r="B5" s="13" t="s">
         <v>2</v>
       </c>
@@ -794,10 +872,20 @@
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
       <c r="K5" s="22"/>
-      <c r="L5" s="15"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="13"/>
+      <c r="L5" s="15">
+        <v>10</v>
+      </c>
+      <c r="M5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>36</v>
+      </c>
+      <c r="B6" s="13">
+        <v>28</v>
+      </c>
       <c r="C6" s="21"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -807,10 +895,20 @@
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="22"/>
-      <c r="L6" s="15"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="13"/>
+      <c r="L6" s="15">
+        <v>11</v>
+      </c>
+      <c r="M6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>35</v>
+      </c>
+      <c r="B7" s="13">
+        <v>27</v>
+      </c>
       <c r="C7" s="21"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
@@ -820,10 +918,20 @@
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="22"/>
-      <c r="L7" s="15"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="13"/>
+      <c r="L7" s="15">
+        <v>12</v>
+      </c>
+      <c r="M7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>34</v>
+      </c>
+      <c r="B8" s="13">
+        <v>26</v>
+      </c>
       <c r="C8" s="21"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
@@ -836,9 +944,17 @@
       <c r="L8" s="15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="13"/>
+      <c r="M8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>33</v>
+      </c>
+      <c r="B9" s="13">
+        <v>25</v>
+      </c>
       <c r="C9" s="21"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -851,9 +967,17 @@
       <c r="L9" s="15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="13"/>
+      <c r="M9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>32</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>20</v>
+      </c>
       <c r="C10" s="21"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -863,10 +987,20 @@
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="22"/>
-      <c r="L10" s="15"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="13"/>
+      <c r="L10" s="15">
+        <v>13</v>
+      </c>
+      <c r="M10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>31</v>
+      </c>
+      <c r="B11" s="13">
+        <v>23</v>
+      </c>
       <c r="C11" s="23"/>
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
@@ -876,74 +1010,94 @@
       <c r="I11" s="24"/>
       <c r="J11" s="24"/>
       <c r="K11" s="25"/>
-      <c r="L11" s="15"/>
-    </row>
-    <row r="12" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
+      <c r="L11" s="15">
+        <v>14</v>
+      </c>
+      <c r="M11">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="8">
+        <v>22</v>
+      </c>
       <c r="C12" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="11"/>
+      <c r="D12" s="11">
+        <v>21</v>
+      </c>
       <c r="E12" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
+      <c r="F12" s="11">
+        <v>20</v>
+      </c>
+      <c r="G12" s="11">
+        <v>19</v>
+      </c>
       <c r="H12" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="7"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="I12" s="11">
+        <v>18</v>
+      </c>
+      <c r="J12" s="11">
+        <v>17</v>
+      </c>
+      <c r="K12" s="10">
+        <v>16</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <v>29</v>
+      </c>
+      <c r="D13">
+        <v>28</v>
+      </c>
+      <c r="E13">
+        <v>27</v>
+      </c>
+      <c r="F13">
+        <v>26</v>
+      </c>
+      <c r="G13">
+        <v>25</v>
+      </c>
+      <c r="H13">
+        <v>24</v>
+      </c>
+      <c r="I13">
+        <v>23</v>
+      </c>
+      <c r="J13">
+        <v>22</v>
+      </c>
+      <c r="K13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
         <v>1</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="4">
-        <v>2</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="4">
-        <v>3</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -956,48 +1110,48 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
+        <v>2</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>3</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
         <v>4</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B19" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
-        <v>5</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
-        <v>6</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -1010,12 +1164,12 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -1028,12 +1182,12 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -1046,12 +1200,12 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -1064,12 +1218,12 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -1082,12 +1236,12 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -1100,12 +1254,12 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -1118,12 +1272,12 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -1136,21 +1290,421 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
     </row>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
+        <v>12</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+    </row>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
+        <v>13</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+    </row>
+    <row r="29" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
+        <v>14</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+    </row>
+    <row r="30" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>15</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+    </row>
+    <row r="32" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>3</v>
+      </c>
+      <c r="G32">
+        <v>4</v>
+      </c>
+      <c r="H32">
+        <v>5</v>
+      </c>
+      <c r="I32">
+        <v>6</v>
+      </c>
+      <c r="J32">
+        <v>7</v>
+      </c>
+      <c r="K32">
+        <v>8</v>
+      </c>
+      <c r="L32">
+        <v>9</v>
+      </c>
+      <c r="M32">
+        <v>10</v>
+      </c>
+      <c r="N32">
+        <v>11</v>
+      </c>
+      <c r="O32">
+        <v>12</v>
+      </c>
+      <c r="P32">
+        <v>13</v>
+      </c>
+      <c r="Q32">
+        <v>14</v>
+      </c>
+      <c r="R32">
+        <v>15</v>
+      </c>
+      <c r="S32">
+        <v>16</v>
+      </c>
+      <c r="T32">
+        <v>17</v>
+      </c>
+      <c r="U32">
+        <v>18</v>
+      </c>
+      <c r="V32">
+        <v>19</v>
+      </c>
+      <c r="W32">
+        <v>20</v>
+      </c>
+      <c r="X32">
+        <v>21</v>
+      </c>
+      <c r="Y32">
+        <v>22</v>
+      </c>
+      <c r="Z32">
+        <v>23</v>
+      </c>
+      <c r="AA32">
+        <v>24</v>
+      </c>
+      <c r="AB32">
+        <v>25</v>
+      </c>
+      <c r="AC32">
+        <v>26</v>
+      </c>
+      <c r="AD32">
+        <v>27</v>
+      </c>
+      <c r="AE32">
+        <v>28</v>
+      </c>
+      <c r="AF32">
+        <v>29</v>
+      </c>
+      <c r="AG32">
+        <v>30</v>
+      </c>
+      <c r="AH32">
+        <v>31</v>
+      </c>
+      <c r="AI32">
+        <v>32</v>
+      </c>
+      <c r="AJ32">
+        <v>33</v>
+      </c>
+      <c r="AK32">
+        <v>34</v>
+      </c>
+      <c r="AL32">
+        <v>35</v>
+      </c>
+      <c r="AM32">
+        <v>36</v>
+      </c>
+      <c r="AN32">
+        <v>37</v>
+      </c>
+      <c r="AO32">
+        <v>38</v>
+      </c>
+      <c r="AP32">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B39">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B42">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B44">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B46">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B47">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B48">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B49">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B50">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B51">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B52">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B53">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B54">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B55">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B56">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B57">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B58">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B59">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B60">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B61">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B62">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B63">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B64">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B65">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B66">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B67">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B68">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B69">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B70">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B71">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B72">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="B26:L26"/>
-    <mergeCell ref="B20:L20"/>
-    <mergeCell ref="B21:L21"/>
+  <mergeCells count="15">
+    <mergeCell ref="B28:L28"/>
+    <mergeCell ref="B29:M29"/>
+    <mergeCell ref="B30:O30"/>
     <mergeCell ref="B22:L22"/>
     <mergeCell ref="B23:L23"/>
     <mergeCell ref="B24:L24"/>
     <mergeCell ref="B25:L25"/>
-    <mergeCell ref="B14:L14"/>
-    <mergeCell ref="B15:L15"/>
+    <mergeCell ref="B26:L26"/>
+    <mergeCell ref="B27:L27"/>
     <mergeCell ref="B16:L16"/>
     <mergeCell ref="B17:L17"/>
     <mergeCell ref="B18:L18"/>
     <mergeCell ref="B19:L19"/>
+    <mergeCell ref="B20:L20"/>
+    <mergeCell ref="B21:L21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finished documentation and analysis
</commit_message>
<xml_diff>
--- a/IOBgamemap.xlsx
+++ b/IOBgamemap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Oliver/Desktop/NEU/IS6105/001443089_001498905_6_Zhe_Xu_Yixin_Guo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6652E342-346E-8B4B-BCDB-598DEFD4CE8F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6F53E7-526C-CF4C-A1DB-46D045F06FCD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{75293F48-95FD-CA44-BED8-E365127A4EB5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{75293F48-95FD-CA44-BED8-E365127A4EB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>Garlic Garden</t>
   </si>
   <si>
-    <t>Infinity Outlast Battle</t>
-  </si>
-  <si>
     <t>Rules</t>
   </si>
   <si>
@@ -100,6 +97,9 @@
   </si>
   <si>
     <t>Chance cards: there are 2 chance cards, 1 of them is "the key" for the player to get out of Diagon Alley, the other one traps player for this current roll</t>
+  </si>
+  <si>
+    <t>Infinite Outlast Battle</t>
   </si>
 </sst>
 </file>
@@ -355,11 +355,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -402,6 +400,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="60% - Accent3" xfId="1" builtinId="40"/>
@@ -720,7 +720,7 @@
   <dimension ref="A1:AP72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:O30"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -733,13 +733,13 @@
     <col min="9" max="9" width="12.5" customWidth="1"/>
     <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.83203125" style="9" customWidth="1"/>
-    <col min="15" max="23" width="10.83203125" style="9"/>
+    <col min="14" max="14" width="10.83203125" style="7" customWidth="1"/>
+    <col min="15" max="23" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -779,34 +779,34 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="14">
         <v>1</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2" s="14">
         <v>2</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="15">
         <v>3</v>
       </c>
-      <c r="G2" s="16">
+      <c r="G2" s="14">
         <v>4</v>
       </c>
-      <c r="H2" s="17">
+      <c r="H2" s="15">
         <v>5</v>
       </c>
-      <c r="I2" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="16">
+      <c r="I2" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="14">
         <v>7</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -814,19 +814,19 @@
       <c r="A3">
         <v>39</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="10">
         <v>29</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="14">
+      <c r="C3" s="16"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="12">
         <v>8</v>
       </c>
       <c r="M3">
@@ -837,19 +837,19 @@
       <c r="A4">
         <v>38</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="14">
+      <c r="C4" s="19"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="12">
         <v>9</v>
       </c>
       <c r="M4">
@@ -860,19 +860,19 @@
       <c r="A5">
         <v>37</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="15">
+      <c r="C5" s="19"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="13">
         <v>10</v>
       </c>
       <c r="M5">
@@ -883,19 +883,19 @@
       <c r="A6">
         <v>36</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="11">
         <v>28</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="15">
+      <c r="C6" s="19"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="13">
         <v>11</v>
       </c>
       <c r="M6">
@@ -906,19 +906,19 @@
       <c r="A7">
         <v>35</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="11">
         <v>27</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="15">
+      <c r="C7" s="19"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="13">
         <v>12</v>
       </c>
       <c r="M7">
@@ -929,19 +929,19 @@
       <c r="A8">
         <v>34</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="11">
         <v>26</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="15" t="s">
+      <c r="C8" s="19"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="13" t="s">
         <v>1</v>
       </c>
       <c r="M8">
@@ -952,19 +952,19 @@
       <c r="A9">
         <v>33</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="11">
         <v>25</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="15" t="s">
+      <c r="C9" s="19"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="13" t="s">
         <v>4</v>
       </c>
       <c r="M9">
@@ -975,19 +975,19 @@
       <c r="A10">
         <v>32</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="15">
+      <c r="B10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="13">
         <v>13</v>
       </c>
       <c r="M10">
@@ -998,19 +998,19 @@
       <c r="A11">
         <v>31</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="11">
         <v>23</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="15">
+      <c r="C11" s="21"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="13">
         <v>14</v>
       </c>
       <c r="M11">
@@ -1018,38 +1018,38 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="8">
+      <c r="B12" s="6">
         <v>22</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="9">
         <v>21</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="9">
         <v>20</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="9">
         <v>19</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="9">
         <v>18</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="9">
         <v>17</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12" s="8">
         <v>16</v>
       </c>
-      <c r="L12" s="7" t="s">
-        <v>20</v>
+      <c r="L12" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="M12">
         <v>20</v>
@@ -1088,283 +1088,283 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>1</v>
+      </c>
+      <c r="B16" s="25" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="4">
-        <v>1</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>2</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>3</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="25"/>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>4</v>
+      </c>
+      <c r="B19" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-    </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
-        <v>2</v>
-      </c>
-      <c r="B17" s="3" t="s">
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>5</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>6</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>7</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+    </row>
+    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>8</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+    </row>
+    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>9</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+    </row>
+    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>10</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="24"/>
+    </row>
+    <row r="26" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>11</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+    </row>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>12</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
+      <c r="L27" s="24"/>
+    </row>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <v>13</v>
+      </c>
+      <c r="B28" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
-        <v>3</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-    </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
-        <v>4</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-    </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
-        <v>5</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-    </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
-        <v>6</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-    </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
-        <v>7</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-    </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
-        <v>8</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-    </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
-        <v>9</v>
-      </c>
-      <c r="B24" s="5" t="s">
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+    </row>
+    <row r="29" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
         <v>14</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-    </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
-        <v>10</v>
-      </c>
-      <c r="B25" s="5" t="s">
+      <c r="B29" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
+    </row>
+    <row r="30" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
         <v>15</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-    </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
-        <v>11</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-    </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A27" s="4">
-        <v>12</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-    </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
-        <v>13</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-    </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A29" s="4">
-        <v>14</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-    </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A30" s="4">
-        <v>15</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
+      <c r="B30" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="25"/>
+      <c r="L30" s="25"/>
+      <c r="M30" s="25"/>
+      <c r="N30" s="25"/>
+      <c r="O30" s="25"/>
     </row>
     <row r="32" spans="1:42" x14ac:dyDescent="0.2">
       <c r="C32">
@@ -1690,6 +1690,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B21:L21"/>
+    <mergeCell ref="B16:L16"/>
+    <mergeCell ref="B17:L17"/>
+    <mergeCell ref="B18:L18"/>
+    <mergeCell ref="B19:L19"/>
+    <mergeCell ref="B20:L20"/>
     <mergeCell ref="B28:L28"/>
     <mergeCell ref="B29:M29"/>
     <mergeCell ref="B30:O30"/>
@@ -1699,12 +1705,6 @@
     <mergeCell ref="B25:L25"/>
     <mergeCell ref="B26:L26"/>
     <mergeCell ref="B27:L27"/>
-    <mergeCell ref="B16:L16"/>
-    <mergeCell ref="B17:L17"/>
-    <mergeCell ref="B18:L18"/>
-    <mergeCell ref="B19:L19"/>
-    <mergeCell ref="B20:L20"/>
-    <mergeCell ref="B21:L21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>